<commit_message>
creating part 1 label data processing script
</commit_message>
<xml_diff>
--- a/data/data_digitization/rbcm_data/label_data/raw_data/RBCM-label-entry.xlsx
+++ b/data/data_digitization/rbcm_data/label_data/raw_data/RBCM-label-entry.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/data_digitization/rbcm_data/label_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/data_digitization/rbcm_data/label_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53632C2-1F19-584C-B65B-1B1525BED8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848D593A-A5B3-EF4E-B441-6B40DACA9D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="10320" windowHeight="16880" xr2:uid="{6B6DF4C7-2696-B14D-857F-7620348251C6}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="10320" windowHeight="15400" xr2:uid="{6B6DF4C7-2696-B14D-857F-7620348251C6}"/>
   </bookViews>
   <sheets>
     <sheet name="RBCM-label-entry-template" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>accessionNum</t>
   </si>
   <si>
-    <t>recordNum</t>
-  </si>
-  <si>
     <t>habitatDescription</t>
   </si>
   <si>
@@ -65,27 +62,15 @@
     <t>vlon</t>
   </si>
   <si>
-    <t>V078911</t>
-  </si>
-  <si>
-    <t>V083201</t>
-  </si>
-  <si>
     <t>roadside and meadow; common</t>
   </si>
   <si>
     <t>Mayne Island</t>
   </si>
   <si>
-    <t>V083236</t>
-  </si>
-  <si>
     <t>abandoned farm fields</t>
   </si>
   <si>
-    <t>V083305</t>
-  </si>
-  <si>
     <t>genus</t>
   </si>
   <si>
@@ -98,15 +83,6 @@
     <t xml:space="preserve">millefolium </t>
   </si>
   <si>
-    <t>authority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L. </t>
-  </si>
-  <si>
-    <t>L.</t>
-  </si>
-  <si>
     <t>Daucus</t>
   </si>
   <si>
@@ -119,9 +95,6 @@
     <t xml:space="preserve">vineale </t>
   </si>
   <si>
-    <t>(Nutt.) Coulter &amp; Rose</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lomatium </t>
   </si>
   <si>
@@ -134,18 +107,12 @@
     <t>cernuum</t>
   </si>
   <si>
-    <t>Roth</t>
-  </si>
-  <si>
     <t>dry ridge</t>
   </si>
   <si>
     <t>acuminatum</t>
   </si>
   <si>
-    <t>Hook.</t>
-  </si>
-  <si>
     <t>Mayne Island; Mount Parke</t>
   </si>
   <si>
@@ -161,18 +128,12 @@
     <t>Mayne Island; Horton Bay</t>
   </si>
   <si>
-    <t>777a</t>
-  </si>
-  <si>
     <t xml:space="preserve">Achlys </t>
   </si>
   <si>
     <t>triphylla</t>
   </si>
   <si>
-    <t xml:space="preserve">(Smith) DC. </t>
-  </si>
-  <si>
     <t>moist, Douglas fir - sword ferm forest</t>
   </si>
   <si>
@@ -182,27 +143,18 @@
     <t xml:space="preserve">lemmonii </t>
   </si>
   <si>
-    <t>(Vasey) Scribn.</t>
-  </si>
-  <si>
     <t>open bluffs, widespread in small clumps</t>
   </si>
   <si>
     <t xml:space="preserve">amplectens </t>
   </si>
   <si>
-    <t xml:space="preserve">Torr. </t>
-  </si>
-  <si>
     <t xml:space="preserve">in conglomerate outcrop of Sedum, moss etc. </t>
   </si>
   <si>
     <t>Galiano Island; Mount Sutil</t>
   </si>
   <si>
-    <t>Roth.</t>
-  </si>
-  <si>
     <t>Agrostis</t>
   </si>
   <si>
@@ -218,9 +170,6 @@
     <t xml:space="preserve">utriculatum </t>
   </si>
   <si>
-    <t>(Nutt.) Coult. &amp; Rose</t>
-  </si>
-  <si>
     <t>Galiano Island</t>
   </si>
   <si>
@@ -228,6 +177,21 @@
   </si>
   <si>
     <t>one id revision from Agrostis stolonifera var. stolonifera</t>
+  </si>
+  <si>
+    <t>ssp</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>collNum</t>
+  </si>
+  <si>
+    <t>777A</t>
   </si>
 </sst>
 </file>
@@ -606,422 +570,428 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B8F860-94CC-D344-8430-EBA5B904AFFA}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="106" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="3" width="17" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="7" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="4" max="6" width="6.1640625" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="7" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>78911</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4">
+        <v>26827</v>
+      </c>
+      <c r="L2" s="3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>83201</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="I3" s="3">
+        <v>48</v>
+      </c>
+      <c r="J3" s="3">
+        <v>123</v>
+      </c>
+      <c r="K3" s="4">
+        <v>27610</v>
+      </c>
+      <c r="L3" s="3">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>83236</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="3">
+        <v>48</v>
+      </c>
+      <c r="J4" s="3">
+        <v>123</v>
+      </c>
+      <c r="K4" s="4">
+        <v>27584</v>
+      </c>
+      <c r="L4" s="3">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>83305</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="3">
         <v>48</v>
       </c>
-      <c r="H3" s="3">
+      <c r="J5" s="3">
         <v>123</v>
       </c>
-      <c r="I3" s="4">
-        <v>27610</v>
-      </c>
-      <c r="J3" s="3">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="3">
-        <v>48</v>
-      </c>
-      <c r="H4" s="3">
-        <v>123</v>
-      </c>
-      <c r="I4" s="4">
-        <v>27584</v>
-      </c>
-      <c r="J4" s="3">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="3">
-        <v>48</v>
-      </c>
-      <c r="H5" s="3">
-        <v>123</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="K5" s="4">
         <v>27544</v>
       </c>
-      <c r="J5" s="3">
+      <c r="L5" s="3">
         <v>574</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>83309</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="3">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="3">
         <v>48</v>
       </c>
-      <c r="H6" s="3">
+      <c r="J6" s="3">
         <v>123</v>
       </c>
-      <c r="I6" s="4">
+      <c r="K6" s="4">
         <v>27583</v>
       </c>
-      <c r="J6" s="3">
+      <c r="L6" s="3">
         <v>623</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>83310</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="3">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="3">
         <v>48</v>
       </c>
-      <c r="H7" s="3">
+      <c r="J7" s="3">
         <v>123</v>
       </c>
-      <c r="I7" s="4">
+      <c r="K7" s="4">
         <v>27583</v>
       </c>
-      <c r="J7" s="3">
+      <c r="L7" s="3">
         <v>633</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>83318</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="3">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="3">
         <v>48</v>
       </c>
-      <c r="H8" s="3">
+      <c r="J8" s="3">
         <v>123</v>
       </c>
-      <c r="I8" s="4">
+      <c r="K8" s="4">
         <v>27610</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>83434</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="3">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="3">
         <v>48</v>
       </c>
-      <c r="H9" s="3">
+      <c r="J9" s="3">
         <v>123</v>
       </c>
-      <c r="I9" s="4">
+      <c r="K9" s="4">
         <v>27542</v>
       </c>
-      <c r="J9" s="3">
+      <c r="L9" s="3">
         <v>493</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>87220</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="4">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="4">
         <v>27899</v>
       </c>
-      <c r="J10" s="3">
+      <c r="L10" s="3">
         <v>834</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>87223</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="4">
+        <v>36</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="4">
         <v>27954</v>
       </c>
-      <c r="J11" s="3">
+      <c r="L11" s="3">
         <v>899</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>95478</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="4">
+        <v>40</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4">
         <v>27220</v>
       </c>
-      <c r="J12" s="3">
+      <c r="L12" s="3">
         <v>384</v>
       </c>
-      <c r="K12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="M12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>97110</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="4">
+      <c r="H13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="4">
         <v>27573</v>
       </c>
-      <c r="J13" s="3">
+      <c r="L13" s="3">
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1032,8 +1002,10 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1044,8 +1016,10 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1056,8 +1030,10 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1068,8 +1044,10 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1080,8 +1058,10 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1092,8 +1072,10 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1104,6 +1086,8 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
left over hanges from jan
</commit_message>
<xml_diff>
--- a/data/data_digitization/rbcm_data/label_data/raw_data/RBCM-label-entry.xlsx
+++ b/data/data_digitization/rbcm_data/label_data/raw_data/RBCM-label-entry.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/data_digitization/rbcm_data/label_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848D593A-A5B3-EF4E-B441-6B40DACA9D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F45A2BF-712D-AB41-830A-E5BF89572A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="10320" windowHeight="15400" xr2:uid="{6B6DF4C7-2696-B14D-857F-7620348251C6}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="10320" windowHeight="15320" xr2:uid="{6B6DF4C7-2696-B14D-857F-7620348251C6}"/>
   </bookViews>
   <sheets>
     <sheet name="RBCM-label-entry-template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -128,6 +128,9 @@
     <t>Mayne Island; Horton Bay</t>
   </si>
   <si>
+    <t>777a</t>
+  </si>
+  <si>
     <t xml:space="preserve">Achlys </t>
   </si>
   <si>
@@ -189,9 +192,6 @@
   </si>
   <si>
     <t>collNum</t>
-  </si>
-  <si>
-    <t>777A</t>
   </si>
 </sst>
 </file>
@@ -572,9 +572,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B8F860-94CC-D344-8430-EBA5B904AFFA}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="106" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="135" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,13 +601,13 @@
         <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
@@ -625,10 +625,10 @@
         <v>5</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -846,7 +846,7 @@
         <v>27610</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -854,16 +854,16 @@
         <v>83434</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>9</v>
@@ -886,16 +886,16 @@
         <v>87220</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>4</v>
@@ -917,16 +917,16 @@
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -942,13 +942,13 @@
         <v>95478</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>4</v>
@@ -962,7 +962,7 @@
         <v>384</v>
       </c>
       <c r="M12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -970,17 +970,17 @@
         <v>97110</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>

</xml_diff>